<commit_message>
Fixed an error when trying to merge tables with categorical linking columns
</commit_message>
<xml_diff>
--- a/QSSD/testing/Perfect1-5.xlsx
+++ b/QSSD/testing/Perfect1-5.xlsx
@@ -14,45 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
     <t>Department</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Fred</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>Terry</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>Josh</t>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>£35,000</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>£50,000</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>£45,000</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>Brown</t>
@@ -64,18 +88,51 @@
     <t>Wilson</t>
   </si>
   <si>
+    <t>Ben.Jones@mail.com</t>
+  </si>
+  <si>
+    <t>Fred.Smith@mail.com</t>
+  </si>
+  <si>
+    <t>Tony.Davis@mail.com</t>
+  </si>
+  <si>
+    <t>Terry.Johnson@mail.com</t>
+  </si>
+  <si>
+    <t>Josh.Brown@mail.com</t>
+  </si>
+  <si>
+    <t>JordanWilson@mail.com</t>
+  </si>
+  <si>
+    <t>William.Williams@mail.com</t>
+  </si>
+  <si>
+    <t>Mike.Miller@mail.com</t>
+  </si>
+  <si>
     <t>William</t>
   </si>
   <si>
+    <t>Gareth.Taylor@mail.com</t>
+  </si>
+  <si>
     <t>Willaims</t>
   </si>
   <si>
+    <t>John.Thompson@mail.com</t>
+  </si>
+  <si>
     <t>Mike</t>
   </si>
   <si>
     <t>Miller</t>
   </si>
   <si>
+    <t>Nick.Anderson@mail.com</t>
+  </si>
+  <si>
     <t>Gareth</t>
   </si>
   <si>
@@ -94,64 +151,10 @@
     <t>Anderson</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>£35,000</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>£50,000</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Ben.Jones@mail.com</t>
-  </si>
-  <si>
-    <t>Fred.Smith@mail.com</t>
-  </si>
-  <si>
-    <t>Tony.Davis@mail.com</t>
-  </si>
-  <si>
-    <t>Terry.Johnson@mail.com</t>
-  </si>
-  <si>
-    <t>Josh.Brown@mail.com</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
     <t>£40,000</t>
-  </si>
-  <si>
-    <t>JordanWilson@mail.com</t>
-  </si>
-  <si>
-    <t>William.Williams@mail.com</t>
-  </si>
-  <si>
-    <t>Mike.Miller@mail.com</t>
-  </si>
-  <si>
-    <t>Gareth.Taylor@mail.com</t>
-  </si>
-  <si>
-    <t>John.Thompson@mail.com</t>
-  </si>
-  <si>
-    <t>Nick.Anderson@mail.com</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -213,6 +216,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,10 +453,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -458,10 +464,10 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -469,10 +475,10 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -480,10 +486,10 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +497,10 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -502,10 +508,10 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -513,10 +519,10 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -524,10 +530,10 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -535,10 +541,10 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -546,10 +552,10 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -557,10 +563,10 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -568,10 +574,10 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -591,46 +597,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="5">
-        <v>45000.0</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -668,6 +674,20 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="6"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -692,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -701,7 +721,7 @@
         <v>0.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -710,7 +730,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -719,7 +739,7 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -728,7 +748,7 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -737,7 +757,7 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -746,7 +766,7 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -755,7 +775,7 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -764,7 +784,7 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -773,7 +793,7 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -782,7 +802,7 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -791,7 +811,7 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -812,134 +832,134 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>